<commit_message>
survival and birth, output file
</commit_message>
<xml_diff>
--- a/CAB201_2020S2_ProjectPartB_n10454012/CRA_SoC.xlsx
+++ b/CAB201_2020S2_ProjectPartB_n10454012/CRA_SoC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n10454012\Desktop\CAB201_2020S2_ProjectPartB_n10454012\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chilla/Desktop/game-of-life/CAB201_2020S2_ProjectPartB_n10454012/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41B1E86-B4A2-463C-9A18-F13E8626DFD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED2412F-B291-CA4C-9BF3-8250798B83DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6904C73-38EA-4A0D-987E-F2DCB498C39B}"/>
+    <workbookView xWindow="920" yWindow="500" windowWidth="37480" windowHeight="23500" xr2:uid="{B6904C73-38EA-4A0D-987E-F2DCB498C39B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1411,14 +1420,72 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1429,87 +1496,156 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1519,14 +1655,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1535,160 +1668,36 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2002,50 +2011,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F17C300-24F0-4A87-A928-5249CE4891A5}">
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="3" width="7.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="8" max="9" width="6.42578125" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="9" width="6.5" customWidth="1"/>
+    <col min="10" max="10" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
@@ -2057,7 +2066,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="4" t="s">
@@ -2073,7 +2082,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="4" t="s">
@@ -2087,14 +2096,14 @@
       <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="102">
+      <c r="H5" s="78">
         <f>MIN(SUM(I19,I46,I65,I78),SUM(H19,H46,H65,H78))</f>
-        <v>25</v>
-      </c>
-      <c r="I5" s="103"/>
+        <v>93.5</v>
+      </c>
+      <c r="I5" s="79"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
@@ -2108,14 +2117,14 @@
       <c r="G6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="104">
+      <c r="H6" s="80">
         <f>(H5/100)*0.35</f>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="I6" s="105"/>
+        <v>0.32724999999999999</v>
+      </c>
+      <c r="I6" s="81"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
@@ -2127,21 +2136,21 @@
       <c r="I7" s="20"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="110"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="91"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
@@ -2153,48 +2162,48 @@
       <c r="I9" s="13"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="53" t="s">
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="55" t="s">
+      <c r="I10" s="40" t="s">
         <v>8</v>
       </c>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="107"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="88"/>
       <c r="H12" s="22">
         <v>5</v>
       </c>
@@ -2203,16 +2212,16 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="85"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="49"/>
       <c r="H13" s="24">
         <v>1</v>
       </c>
@@ -2221,16 +2230,16 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
-      <c r="B14" s="83" t="s">
+      <c r="B14" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="85"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="24">
         <v>2</v>
       </c>
@@ -2239,85 +2248,93 @@
       </c>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="92" t="s">
+      <c r="C15" s="97"/>
+      <c r="D15" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="92"/>
-      <c r="F15" s="92"/>
-      <c r="G15" s="93"/>
-      <c r="H15" s="24"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="24">
+        <v>3</v>
+      </c>
       <c r="I15" s="25">
         <v>3</v>
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="92" t="s">
+      <c r="B16" s="98"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="102" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="24"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="24">
+        <v>3</v>
+      </c>
       <c r="I16" s="25">
         <v>3</v>
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="92" t="s">
+      <c r="B17" s="98"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="92"/>
-      <c r="F17" s="92"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="24"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="24">
+        <v>3</v>
+      </c>
       <c r="I17" s="25">
         <v>3</v>
       </c>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="90"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="94" t="s">
+      <c r="B18" s="100"/>
+      <c r="C18" s="101"/>
+      <c r="D18" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="94"/>
-      <c r="F18" s="94"/>
-      <c r="G18" s="95"/>
-      <c r="H18" s="26"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="26">
+        <v>3</v>
+      </c>
       <c r="I18" s="31">
         <v>3</v>
       </c>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="97"/>
-      <c r="D19" s="97"/>
-      <c r="E19" s="97"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="97"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
       <c r="H19" s="14">
         <f>SUM(H12:H18)</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I19" s="15">
         <f>SUM(I12:I18)</f>
@@ -2325,33 +2342,33 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="61"/>
+      <c r="C20" s="111"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="111"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="111"/>
+      <c r="I20" s="112"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
-      <c r="B21" s="68"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="70"/>
+      <c r="B21" s="113"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="114"/>
+      <c r="E21" s="114"/>
+      <c r="F21" s="114"/>
+      <c r="G21" s="114"/>
+      <c r="H21" s="114"/>
+      <c r="I21" s="115"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -2363,50 +2380,50 @@
       <c r="I22" s="13"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53" t="s">
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="55" t="s">
+      <c r="I23" s="40" t="s">
         <v>8</v>
       </c>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="56"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="119"/>
+      <c r="F24" s="119"/>
+      <c r="G24" s="119"/>
+      <c r="H24" s="116"/>
+      <c r="I24" s="117"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
-      <c r="B25" s="79" t="s">
+      <c r="B25" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="80"/>
-      <c r="D25" s="76" t="s">
+      <c r="C25" s="51"/>
+      <c r="D25" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="78"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="88"/>
       <c r="H25" s="22">
         <v>2</v>
       </c>
@@ -2415,34 +2432,36 @@
       </c>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="62" t="s">
+      <c r="B26" s="52"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="27"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="109"/>
+      <c r="H26" s="27">
+        <v>2</v>
+      </c>
       <c r="I26" s="31">
         <v>2</v>
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="80"/>
-      <c r="D27" s="76" t="s">
+      <c r="C27" s="51"/>
+      <c r="D27" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="77"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="78"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="88"/>
       <c r="H27" s="22">
         <v>1</v>
       </c>
@@ -2451,16 +2470,16 @@
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="71" t="s">
+      <c r="B28" s="52"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="73"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="94"/>
       <c r="H28" s="28">
         <v>1</v>
       </c>
@@ -2469,16 +2488,16 @@
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="71" t="s">
+      <c r="B29" s="52"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="73"/>
+      <c r="E29" s="93"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="94"/>
       <c r="H29" s="28">
         <v>1</v>
       </c>
@@ -2487,48 +2506,52 @@
       </c>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
-      <c r="B30" s="81"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="71" t="s">
+      <c r="B30" s="52"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="28"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="28">
+        <v>1</v>
+      </c>
       <c r="I30" s="29">
         <v>1</v>
       </c>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
-      <c r="B31" s="81"/>
-      <c r="C31" s="82"/>
-      <c r="D31" s="71" t="s">
+      <c r="B31" s="52"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="72"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="28"/>
+      <c r="E31" s="93"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="28">
+        <v>1</v>
+      </c>
       <c r="I31" s="29">
         <v>1</v>
       </c>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
-      <c r="B32" s="81"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="71" t="s">
+      <c r="B32" s="52"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="73"/>
+      <c r="E32" s="93"/>
+      <c r="F32" s="93"/>
+      <c r="G32" s="94"/>
       <c r="H32" s="28">
         <v>1</v>
       </c>
@@ -2537,18 +2560,18 @@
       </c>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="80"/>
-      <c r="D33" s="45" t="s">
+      <c r="C33" s="51"/>
+      <c r="D33" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="47"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="65"/>
       <c r="H33" s="22">
         <v>2</v>
       </c>
@@ -2557,16 +2580,16 @@
       </c>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="82"/>
-      <c r="D34" s="65" t="s">
+      <c r="B34" s="52"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="66"/>
-      <c r="F34" s="66"/>
-      <c r="G34" s="67"/>
+      <c r="E34" s="72"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="73"/>
       <c r="H34" s="28">
         <v>2</v>
       </c>
@@ -2575,16 +2598,16 @@
       </c>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
-      <c r="B35" s="81"/>
-      <c r="C35" s="82"/>
-      <c r="D35" s="65" t="s">
+      <c r="B35" s="52"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="106" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="66"/>
-      <c r="F35" s="66"/>
-      <c r="G35" s="67"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="73"/>
       <c r="H35" s="28">
         <v>2</v>
       </c>
@@ -2593,68 +2616,74 @@
       </c>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
-      <c r="B36" s="81"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="83" t="s">
+      <c r="B36" s="52"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="84"/>
-      <c r="F36" s="84"/>
-      <c r="G36" s="85"/>
-      <c r="H36" s="28"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="28">
+        <v>2</v>
+      </c>
       <c r="I36" s="29">
         <v>2</v>
       </c>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
-      <c r="B37" s="81"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="83" t="s">
+      <c r="B37" s="52"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="E37" s="84"/>
-      <c r="F37" s="84"/>
-      <c r="G37" s="85"/>
-      <c r="H37" s="28"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="28">
+        <v>2</v>
+      </c>
       <c r="I37" s="29">
         <v>2</v>
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
-      <c r="B38" s="81"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="83" t="s">
+      <c r="B38" s="52"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="E38" s="84"/>
-      <c r="F38" s="84"/>
-      <c r="G38" s="85"/>
-      <c r="H38" s="28"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="28">
+        <v>2</v>
+      </c>
       <c r="I38" s="29">
         <v>2</v>
       </c>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
-      <c r="B39" s="79" t="s">
+      <c r="B39" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="80"/>
-      <c r="D39" s="117" t="s">
+      <c r="C39" s="51"/>
+      <c r="D39" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="46" t="s">
+      <c r="E39" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="F39" s="46"/>
-      <c r="G39" s="47"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="65"/>
       <c r="H39" s="22">
         <v>1</v>
       </c>
@@ -2663,16 +2692,16 @@
       </c>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
-      <c r="B40" s="81"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="120" t="s">
+      <c r="B40" s="52"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="F40" s="120"/>
-      <c r="G40" s="121"/>
+      <c r="F40" s="66"/>
+      <c r="G40" s="67"/>
       <c r="H40" s="24">
         <v>1</v>
       </c>
@@ -2681,16 +2710,16 @@
       </c>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
-      <c r="B41" s="81"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="119"/>
-      <c r="E41" s="122" t="s">
+      <c r="B41" s="52"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="F41" s="122"/>
-      <c r="G41" s="123"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="69"/>
       <c r="H41" s="28">
         <v>1</v>
       </c>
@@ -2699,85 +2728,89 @@
       </c>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
-      <c r="B42" s="81"/>
-      <c r="C42" s="82"/>
-      <c r="D42" s="124" t="s">
+      <c r="B42" s="52"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="66" t="s">
+      <c r="E42" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F42" s="66"/>
-      <c r="G42" s="67"/>
+      <c r="F42" s="72"/>
+      <c r="G42" s="73"/>
       <c r="H42" s="28"/>
       <c r="I42" s="29">
         <v>1</v>
       </c>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
-      <c r="B43" s="81"/>
-      <c r="C43" s="82"/>
-      <c r="D43" s="125"/>
-      <c r="E43" s="66" t="s">
+      <c r="B43" s="52"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="F43" s="66"/>
-      <c r="G43" s="67"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="73"/>
       <c r="H43" s="28"/>
       <c r="I43" s="29">
         <v>1</v>
       </c>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
-      <c r="B44" s="81"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="71" t="s">
+      <c r="B44" s="52"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="E44" s="72"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="28"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="28">
+        <v>1</v>
+      </c>
       <c r="I44" s="29">
         <v>1</v>
       </c>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
-      <c r="B45" s="81"/>
-      <c r="C45" s="82"/>
-      <c r="D45" s="71" t="s">
+      <c r="B45" s="52"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="72"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="28"/>
+      <c r="E45" s="93"/>
+      <c r="F45" s="93"/>
+      <c r="G45" s="94"/>
+      <c r="H45" s="28">
+        <v>1</v>
+      </c>
       <c r="I45" s="29">
         <v>1</v>
       </c>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
-      <c r="B46" s="115" t="s">
+      <c r="B46" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="116"/>
-      <c r="D46" s="116"/>
-      <c r="E46" s="116"/>
-      <c r="F46" s="116"/>
-      <c r="G46" s="116"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
       <c r="H46" s="16">
         <f>SUM(H25:H45)</f>
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I46" s="17">
         <f>SUM(I25:I45)</f>
@@ -2785,33 +2818,33 @@
       </c>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
-      <c r="B47" s="59" t="s">
+      <c r="B47" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
-      <c r="I47" s="61"/>
+      <c r="C47" s="111"/>
+      <c r="D47" s="111"/>
+      <c r="E47" s="111"/>
+      <c r="F47" s="111"/>
+      <c r="G47" s="111"/>
+      <c r="H47" s="111"/>
+      <c r="I47" s="112"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="41"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="35"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
@@ -2823,50 +2856,50 @@
       <c r="I49" s="13"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
-      <c r="B50" s="51" t="s">
+      <c r="B50" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="52"/>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="53" t="s">
+      <c r="C50" s="83"/>
+      <c r="D50" s="83"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="83"/>
+      <c r="H50" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="55" t="s">
+      <c r="I50" s="40" t="s">
         <v>8</v>
       </c>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
-      <c r="B51" s="57" t="s">
+      <c r="B51" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="54"/>
-      <c r="I51" s="56"/>
+      <c r="C51" s="85"/>
+      <c r="D51" s="85"/>
+      <c r="E51" s="85"/>
+      <c r="F51" s="85"/>
+      <c r="G51" s="85"/>
+      <c r="H51" s="116"/>
+      <c r="I51" s="117"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
-      <c r="B52" s="79" t="s">
+      <c r="B52" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="C52" s="80"/>
-      <c r="D52" s="42" t="s">
+      <c r="C52" s="51"/>
+      <c r="D52" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="44"/>
+      <c r="E52" s="124"/>
+      <c r="F52" s="124"/>
+      <c r="G52" s="125"/>
       <c r="H52" s="22">
         <v>2</v>
       </c>
@@ -2875,217 +2908,241 @@
       </c>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
-      <c r="B53" s="81"/>
-      <c r="C53" s="82"/>
-      <c r="D53" s="68" t="s">
+      <c r="B53" s="52"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="E53" s="69"/>
-      <c r="F53" s="69"/>
-      <c r="G53" s="70"/>
-      <c r="H53" s="27"/>
+      <c r="E53" s="114"/>
+      <c r="F53" s="114"/>
+      <c r="G53" s="115"/>
+      <c r="H53" s="27">
+        <v>1</v>
+      </c>
       <c r="I53" s="31">
         <v>2</v>
       </c>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
-      <c r="B54" s="81"/>
-      <c r="C54" s="82"/>
-      <c r="D54" s="33" t="s">
+      <c r="B54" s="52"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="27"/>
+      <c r="E54" s="121"/>
+      <c r="F54" s="121"/>
+      <c r="G54" s="122"/>
+      <c r="H54" s="27">
+        <v>2</v>
+      </c>
       <c r="I54" s="31">
         <v>2</v>
       </c>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
-      <c r="B55" s="81"/>
-      <c r="C55" s="82"/>
-      <c r="D55" s="48" t="s">
+      <c r="B55" s="52"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="126" t="s">
         <v>77</v>
       </c>
-      <c r="E55" s="49"/>
-      <c r="F55" s="49"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="26"/>
+      <c r="E55" s="127"/>
+      <c r="F55" s="127"/>
+      <c r="G55" s="128"/>
+      <c r="H55" s="26">
+        <v>2</v>
+      </c>
       <c r="I55" s="31">
         <v>2</v>
       </c>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
-      <c r="B56" s="79" t="s">
+      <c r="B56" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="80"/>
-      <c r="D56" s="45" t="s">
+      <c r="C56" s="51"/>
+      <c r="D56" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="E56" s="46"/>
-      <c r="F56" s="46"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="22"/>
+      <c r="E56" s="64"/>
+      <c r="F56" s="64"/>
+      <c r="G56" s="65"/>
+      <c r="H56" s="22">
+        <v>1</v>
+      </c>
       <c r="I56" s="23">
         <v>1</v>
       </c>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
-      <c r="B57" s="81"/>
-      <c r="C57" s="82"/>
-      <c r="D57" s="36" t="s">
+      <c r="B57" s="52"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="38"/>
-      <c r="H57" s="24"/>
+      <c r="E57" s="59"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="24">
+        <v>1</v>
+      </c>
       <c r="I57" s="25">
         <v>1</v>
       </c>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5"/>
-      <c r="B58" s="111"/>
-      <c r="C58" s="112"/>
-      <c r="D58" s="39" t="s">
+      <c r="B58" s="54"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="26"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="26">
+        <v>1</v>
+      </c>
       <c r="I58" s="32">
         <v>2</v>
       </c>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
-      <c r="B59" s="79" t="s">
+      <c r="B59" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="80"/>
-      <c r="D59" s="45" t="s">
+      <c r="C59" s="51"/>
+      <c r="D59" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="E59" s="46"/>
-      <c r="F59" s="46"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="22"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="22">
+        <v>5</v>
+      </c>
       <c r="I59" s="23">
         <v>5</v>
       </c>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
-      <c r="B60" s="81"/>
-      <c r="C60" s="82"/>
-      <c r="D60" s="36" t="s">
+      <c r="B60" s="52"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="E60" s="37"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="24"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="60"/>
+      <c r="H60" s="24">
+        <v>5</v>
+      </c>
       <c r="I60" s="25">
         <v>5</v>
       </c>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
-      <c r="B61" s="81"/>
-      <c r="C61" s="82"/>
-      <c r="D61" s="36" t="s">
+      <c r="B61" s="52"/>
+      <c r="C61" s="53"/>
+      <c r="D61" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="38"/>
-      <c r="H61" s="24"/>
+      <c r="E61" s="59"/>
+      <c r="F61" s="59"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="24">
+        <v>2.5</v>
+      </c>
       <c r="I61" s="25">
         <v>5</v>
       </c>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
-      <c r="B62" s="81"/>
-      <c r="C62" s="82"/>
-      <c r="D62" s="62" t="s">
+      <c r="B62" s="52"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="107" t="s">
         <v>72</v>
       </c>
-      <c r="E62" s="63"/>
-      <c r="F62" s="63"/>
-      <c r="G62" s="64"/>
-      <c r="H62" s="27"/>
+      <c r="E62" s="108"/>
+      <c r="F62" s="108"/>
+      <c r="G62" s="109"/>
+      <c r="H62" s="27">
+        <v>3</v>
+      </c>
       <c r="I62" s="31">
         <v>3</v>
       </c>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
-      <c r="B63" s="79" t="s">
+      <c r="B63" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="80"/>
-      <c r="D63" s="33" t="s">
+      <c r="C63" s="51"/>
+      <c r="D63" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="22"/>
+      <c r="E63" s="121"/>
+      <c r="F63" s="121"/>
+      <c r="G63" s="122"/>
+      <c r="H63" s="22">
+        <v>3</v>
+      </c>
       <c r="I63" s="23">
         <v>3</v>
       </c>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
-      <c r="B64" s="111"/>
-      <c r="C64" s="112"/>
-      <c r="D64" s="113" t="s">
+      <c r="B64" s="54"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="E64" s="113"/>
-      <c r="F64" s="113"/>
-      <c r="G64" s="114"/>
-      <c r="H64" s="26"/>
+      <c r="E64" s="56"/>
+      <c r="F64" s="56"/>
+      <c r="G64" s="57"/>
+      <c r="H64" s="26">
+        <v>3</v>
+      </c>
       <c r="I64" s="32">
         <v>3</v>
       </c>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
-      <c r="B65" s="115" t="s">
+      <c r="B65" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C65" s="116"/>
-      <c r="D65" s="116"/>
-      <c r="E65" s="116"/>
-      <c r="F65" s="116"/>
-      <c r="G65" s="116"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
       <c r="H65" s="16">
         <f>SUM(H52:H64)</f>
-        <v>2</v>
+        <v>31.5</v>
       </c>
       <c r="I65" s="17">
         <f>SUM(I52:I64)</f>
@@ -3093,33 +3150,33 @@
       </c>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
-      <c r="B66" s="59" t="s">
+      <c r="B66" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="60"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="60"/>
-      <c r="F66" s="60"/>
-      <c r="G66" s="60"/>
-      <c r="H66" s="60"/>
-      <c r="I66" s="61"/>
+      <c r="C66" s="111"/>
+      <c r="D66" s="111"/>
+      <c r="E66" s="111"/>
+      <c r="F66" s="111"/>
+      <c r="G66" s="111"/>
+      <c r="H66" s="111"/>
+      <c r="I66" s="112"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
-      <c r="B67" s="39"/>
-      <c r="C67" s="40"/>
-      <c r="D67" s="40"/>
-      <c r="E67" s="40"/>
-      <c r="F67" s="40"/>
-      <c r="G67" s="40"/>
-      <c r="H67" s="40"/>
-      <c r="I67" s="41"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="34"/>
+      <c r="F67" s="34"/>
+      <c r="G67" s="34"/>
+      <c r="H67" s="34"/>
+      <c r="I67" s="35"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5"/>
       <c r="B68" s="18"/>
       <c r="C68" s="30"/>
@@ -3131,198 +3188,272 @@
       <c r="I68" s="19"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
-      <c r="B69" s="51" t="s">
+      <c r="B69" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="52"/>
-      <c r="D69" s="52"/>
-      <c r="E69" s="52"/>
-      <c r="F69" s="52"/>
-      <c r="G69" s="52"/>
-      <c r="H69" s="53" t="s">
+      <c r="C69" s="83"/>
+      <c r="D69" s="83"/>
+      <c r="E69" s="83"/>
+      <c r="F69" s="83"/>
+      <c r="G69" s="83"/>
+      <c r="H69" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="I69" s="55" t="s">
+      <c r="I69" s="40" t="s">
         <v>8</v>
       </c>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5"/>
-      <c r="B70" s="57" t="s">
+      <c r="B70" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
-      <c r="F70" s="58"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="106"/>
-      <c r="I70" s="107"/>
+      <c r="C70" s="85"/>
+      <c r="D70" s="85"/>
+      <c r="E70" s="85"/>
+      <c r="F70" s="85"/>
+      <c r="G70" s="85"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="41"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
-      <c r="B71" s="45" t="s">
+      <c r="B71" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="C71" s="46"/>
-      <c r="D71" s="46"/>
-      <c r="E71" s="46"/>
-      <c r="F71" s="46"/>
-      <c r="G71" s="47"/>
-      <c r="H71" s="22"/>
+      <c r="C71" s="64"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="65"/>
+      <c r="H71" s="22">
+        <v>2</v>
+      </c>
       <c r="I71" s="23">
         <v>2</v>
       </c>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
-      <c r="B72" s="65" t="s">
+      <c r="B72" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="C72" s="66"/>
-      <c r="D72" s="66"/>
-      <c r="E72" s="66"/>
-      <c r="F72" s="66"/>
-      <c r="G72" s="67"/>
-      <c r="H72" s="24"/>
+      <c r="C72" s="72"/>
+      <c r="D72" s="72"/>
+      <c r="E72" s="72"/>
+      <c r="F72" s="72"/>
+      <c r="G72" s="73"/>
+      <c r="H72" s="24">
+        <v>1</v>
+      </c>
       <c r="I72" s="25">
         <v>1</v>
       </c>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
-      <c r="B73" s="36" t="s">
+      <c r="B73" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="37"/>
-      <c r="G73" s="38"/>
-      <c r="H73" s="24"/>
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="59"/>
+      <c r="F73" s="59"/>
+      <c r="G73" s="60"/>
+      <c r="H73" s="24">
+        <v>2</v>
+      </c>
       <c r="I73" s="25">
         <v>2</v>
       </c>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5"/>
-      <c r="B74" s="65" t="s">
+      <c r="B74" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="C74" s="66"/>
-      <c r="D74" s="66"/>
-      <c r="E74" s="66"/>
-      <c r="F74" s="66"/>
-      <c r="G74" s="67"/>
-      <c r="H74" s="24"/>
+      <c r="C74" s="72"/>
+      <c r="D74" s="72"/>
+      <c r="E74" s="72"/>
+      <c r="F74" s="72"/>
+      <c r="G74" s="73"/>
+      <c r="H74" s="24">
+        <v>2</v>
+      </c>
       <c r="I74" s="25">
         <v>2</v>
       </c>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
-      <c r="B75" s="65" t="s">
+      <c r="B75" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="C75" s="66"/>
-      <c r="D75" s="66"/>
-      <c r="E75" s="66"/>
-      <c r="F75" s="66"/>
-      <c r="G75" s="67"/>
-      <c r="H75" s="24"/>
+      <c r="C75" s="72"/>
+      <c r="D75" s="72"/>
+      <c r="E75" s="72"/>
+      <c r="F75" s="72"/>
+      <c r="G75" s="73"/>
+      <c r="H75" s="24">
+        <v>3</v>
+      </c>
       <c r="I75" s="25">
         <v>3</v>
       </c>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
-      <c r="B76" s="126" t="s">
+      <c r="B76" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C76" s="127"/>
-      <c r="D76" s="127"/>
-      <c r="E76" s="127"/>
-      <c r="F76" s="127"/>
-      <c r="G76" s="128"/>
-      <c r="H76" s="27"/>
+      <c r="C76" s="45"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="45"/>
+      <c r="F76" s="45"/>
+      <c r="G76" s="46"/>
+      <c r="H76" s="27">
+        <v>2</v>
+      </c>
       <c r="I76" s="31">
         <v>2</v>
       </c>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="126" t="s">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B77" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C77" s="127"/>
-      <c r="D77" s="127"/>
-      <c r="E77" s="127"/>
-      <c r="F77" s="127"/>
-      <c r="G77" s="128"/>
-      <c r="H77" s="26"/>
+      <c r="C77" s="45"/>
+      <c r="D77" s="45"/>
+      <c r="E77" s="45"/>
+      <c r="F77" s="45"/>
+      <c r="G77" s="46"/>
+      <c r="H77" s="26">
+        <v>3</v>
+      </c>
       <c r="I77" s="31">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B78" s="96" t="s">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B78" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C78" s="97"/>
-      <c r="D78" s="97"/>
-      <c r="E78" s="97"/>
-      <c r="F78" s="97"/>
-      <c r="G78" s="97"/>
+      <c r="C78" s="43"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="43"/>
       <c r="H78" s="14">
         <f>SUM(H71:H77)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I78" s="15">
         <f>SUM(I71:I77)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B79" s="59" t="s">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B79" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="60"/>
-      <c r="D79" s="60"/>
-      <c r="E79" s="60"/>
-      <c r="F79" s="60"/>
-      <c r="G79" s="60"/>
-      <c r="H79" s="60"/>
-      <c r="I79" s="61"/>
-    </row>
-    <row r="80" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="39"/>
-      <c r="C80" s="40"/>
-      <c r="D80" s="40"/>
-      <c r="E80" s="40"/>
-      <c r="F80" s="40"/>
-      <c r="G80" s="40"/>
-      <c r="H80" s="40"/>
-      <c r="I80" s="41"/>
+      <c r="C79" s="111"/>
+      <c r="D79" s="111"/>
+      <c r="E79" s="111"/>
+      <c r="F79" s="111"/>
+      <c r="G79" s="111"/>
+      <c r="H79" s="111"/>
+      <c r="I79" s="112"/>
+    </row>
+    <row r="80" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="33"/>
+      <c r="C80" s="34"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="34"/>
+      <c r="G80" s="34"/>
+      <c r="H80" s="34"/>
+      <c r="I80" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="92">
-    <mergeCell ref="B80:I80"/>
-    <mergeCell ref="B65:G65"/>
-    <mergeCell ref="B67:I67"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="B78:G78"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D60:G60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D59:G59"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="I50:I51"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B79:I79"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="B66:I66"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="B74:G74"/>
+    <mergeCell ref="B75:G75"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="B27:C32"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="B15:C18"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B8:I8"/>
     <mergeCell ref="D38:G38"/>
     <mergeCell ref="B52:C55"/>
     <mergeCell ref="B56:C58"/>
@@ -3339,74 +3470,14 @@
     <mergeCell ref="E41:G41"/>
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="E42:G42"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="B15:C18"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="B27:C32"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B48:I48"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="I50:I51"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B79:I79"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="D63:G63"/>
-    <mergeCell ref="B66:I66"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="B74:G74"/>
-    <mergeCell ref="B75:G75"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D60:G60"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="B80:I80"/>
+    <mergeCell ref="B65:G65"/>
+    <mergeCell ref="B67:I67"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="I69:I70"/>
+    <mergeCell ref="B78:G78"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>